<commit_message>
move final programs to separate folder
</commit_message>
<xml_diff>
--- a/Filtered_By_Region/CAR/CAR_GABALDON.xlsx
+++ b/Filtered_By_Region/CAR/CAR_GABALDON.xlsx
@@ -32,12 +32,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -58,14 +64,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -435,2106 +447,2137 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="34" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="23" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
+    <col width="58" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
+    <col width="17" customWidth="1" min="14" max="14"/>
+    <col width="17" customWidth="1" min="15" max="15"/>
+    <col width="26" customWidth="1" min="16" max="16"/>
+    <col width="26" customWidth="1" min="17" max="17"/>
+    <col width="27" customWidth="1" min="18" max="18"/>
+    <col width="22" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="31" customWidth="1" min="21" max="21"/>
+    <col width="27" customWidth="1" min="22" max="22"/>
+    <col width="19" customWidth="1" min="23" max="23"/>
+    <col width="33" customWidth="1" min="24" max="24"/>
+    <col width="31" customWidth="1" min="25" max="25"/>
+    <col width="64" customWidth="1" min="26" max="26"/>
+    <col width="123" customWidth="1" min="27" max="27"/>
+    <col width="28" customWidth="1" min="28" max="28"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>CATEGORY</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>REGION</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>DIVISION</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>SCHOOL ID</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>SCHOOL NAME</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>MUNICIPALITY</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>LD</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>TOTAL NO. OF SITES</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>TOTAL PHYSICAL TARGET</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>TOTAL NO. OF BUILDINGS</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>SCOPE OF WORK</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>PROJECT ALLOCATION</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>BATCH</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>CONTRACT AMOUNT</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>PERCENTAGE OF COMPLETION</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Target Completion Date </t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>Actual Date of Completion</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>Project ID</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>Contract ID</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>Issuance of Invitation to Bid</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>Pre-Submission Conference</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>Bid Opening</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>Issuance of Resolution to Award</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Issuance of Notice to Proceed</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>Name of Contractor</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
         <is>
           <t>Other Remarks</t>
         </is>
       </c>
-      <c r="AB1" s="3" t="inlineStr">
-        <is>
-          <t>Status as of July 4, 2025</t>
+      <c r="AB1" s="4" t="inlineStr">
+        <is>
+          <t>Status as of July 11, 2025</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>134979</v>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>Bangued West CS</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>BANGUED (Capital)</t>
         </is>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="n">
+      <c r="H2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="inlineStr">
+      <c r="J2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="5" t="n">
         <v>3477721.44</v>
       </c>
-      <c r="M2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="4" t="inlineStr"/>
-      <c r="O2" s="4" t="inlineStr">
+      <c r="M2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5" t="inlineStr"/>
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="4" t="inlineStr"/>
-      <c r="R2" s="4" t="inlineStr"/>
-      <c r="S2" s="4" t="inlineStr"/>
-      <c r="T2" s="4" t="inlineStr"/>
-      <c r="U2" s="4" t="inlineStr"/>
-      <c r="V2" s="4" t="inlineStr"/>
-      <c r="W2" s="4" t="inlineStr"/>
-      <c r="X2" s="4" t="inlineStr"/>
-      <c r="Y2" s="4" t="inlineStr"/>
-      <c r="Z2" s="4" t="inlineStr"/>
-      <c r="AA2" s="4" t="inlineStr"/>
-      <c r="AB2" s="4" t="n"/>
+      <c r="P2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5" t="inlineStr"/>
+      <c r="R2" s="5" t="inlineStr"/>
+      <c r="S2" s="5" t="inlineStr"/>
+      <c r="T2" s="5" t="inlineStr"/>
+      <c r="U2" s="5" t="inlineStr"/>
+      <c r="V2" s="5" t="inlineStr"/>
+      <c r="W2" s="5" t="inlineStr"/>
+      <c r="X2" s="5" t="inlineStr"/>
+      <c r="Y2" s="5" t="inlineStr"/>
+      <c r="Z2" s="5" t="inlineStr"/>
+      <c r="AA2" s="5" t="inlineStr"/>
+      <c r="AB2" s="6" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>135397</v>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="5" t="inlineStr">
         <is>
           <t>Topdac ES</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>ATOK</t>
         </is>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4" t="n">
+      <c r="H3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4" t="inlineStr">
+      <c r="J3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="5" t="n">
         <v>12177572.29</v>
       </c>
-      <c r="M3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="4" t="inlineStr"/>
-      <c r="O3" s="4" t="inlineStr">
+      <c r="M3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5" t="inlineStr"/>
+      <c r="O3" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="4" t="inlineStr"/>
-      <c r="R3" s="4" t="inlineStr"/>
-      <c r="S3" s="4" t="inlineStr"/>
-      <c r="T3" s="4" t="inlineStr"/>
-      <c r="U3" s="4" t="inlineStr"/>
-      <c r="V3" s="4" t="inlineStr"/>
-      <c r="W3" s="4" t="inlineStr"/>
-      <c r="X3" s="4" t="inlineStr"/>
-      <c r="Y3" s="4" t="inlineStr"/>
-      <c r="Z3" s="4" t="inlineStr"/>
-      <c r="AA3" s="4" t="inlineStr"/>
-      <c r="AB3" s="4" t="n"/>
+      <c r="P3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5" t="inlineStr"/>
+      <c r="R3" s="5" t="inlineStr"/>
+      <c r="S3" s="5" t="inlineStr"/>
+      <c r="T3" s="5" t="inlineStr"/>
+      <c r="U3" s="5" t="inlineStr"/>
+      <c r="V3" s="5" t="inlineStr"/>
+      <c r="W3" s="5" t="inlineStr"/>
+      <c r="X3" s="5" t="inlineStr"/>
+      <c r="Y3" s="5" t="inlineStr"/>
+      <c r="Z3" s="5" t="inlineStr"/>
+      <c r="AA3" s="5" t="inlineStr"/>
+      <c r="AB3" s="6" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>135737</v>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="5" t="inlineStr">
         <is>
           <t>Tublay Central Elementary School</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>TUBLAY</t>
         </is>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4" t="n">
+      <c r="H4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4" t="inlineStr">
+      <c r="J4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="5" t="n">
         <v>13636660.38</v>
       </c>
-      <c r="M4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="4" t="inlineStr"/>
-      <c r="O4" s="4" t="inlineStr">
+      <c r="M4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5" t="inlineStr"/>
+      <c r="O4" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="4" t="inlineStr"/>
-      <c r="R4" s="4" t="inlineStr"/>
-      <c r="S4" s="4" t="inlineStr"/>
-      <c r="T4" s="4" t="inlineStr"/>
-      <c r="U4" s="4" t="inlineStr"/>
-      <c r="V4" s="4" t="inlineStr"/>
-      <c r="W4" s="4" t="inlineStr"/>
-      <c r="X4" s="4" t="inlineStr"/>
-      <c r="Y4" s="4" t="inlineStr"/>
-      <c r="Z4" s="4" t="inlineStr"/>
-      <c r="AA4" s="4" t="inlineStr"/>
-      <c r="AB4" s="4" t="n"/>
+      <c r="P4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5" t="inlineStr"/>
+      <c r="R4" s="5" t="inlineStr"/>
+      <c r="S4" s="5" t="inlineStr"/>
+      <c r="T4" s="5" t="inlineStr"/>
+      <c r="U4" s="5" t="inlineStr"/>
+      <c r="V4" s="5" t="inlineStr"/>
+      <c r="W4" s="5" t="inlineStr"/>
+      <c r="X4" s="5" t="inlineStr"/>
+      <c r="Y4" s="5" t="inlineStr"/>
+      <c r="Z4" s="5" t="inlineStr"/>
+      <c r="AA4" s="5" t="inlineStr"/>
+      <c r="AB4" s="6" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>136248</v>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>Tambuan Elementary School</t>
         </is>
       </c>
-      <c r="F5" s="4" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>BESAO</t>
         </is>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="n">
+      <c r="H5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4" t="inlineStr">
+      <c r="J5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="5" t="n">
         <v>12055183.04</v>
       </c>
-      <c r="M5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4" t="inlineStr"/>
-      <c r="O5" s="4" t="inlineStr">
+      <c r="M5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5" t="inlineStr"/>
+      <c r="O5" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="4" t="inlineStr"/>
-      <c r="R5" s="4" t="inlineStr"/>
-      <c r="S5" s="4" t="inlineStr"/>
-      <c r="T5" s="4" t="inlineStr"/>
-      <c r="U5" s="4" t="inlineStr"/>
-      <c r="V5" s="4" t="inlineStr"/>
-      <c r="W5" s="4" t="inlineStr"/>
-      <c r="X5" s="4" t="inlineStr"/>
-      <c r="Y5" s="4" t="inlineStr"/>
-      <c r="Z5" s="4" t="inlineStr"/>
-      <c r="AA5" s="4" t="inlineStr"/>
-      <c r="AB5" s="4" t="n"/>
+      <c r="P5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5" t="inlineStr"/>
+      <c r="R5" s="5" t="inlineStr"/>
+      <c r="S5" s="5" t="inlineStr"/>
+      <c r="T5" s="5" t="inlineStr"/>
+      <c r="U5" s="5" t="inlineStr"/>
+      <c r="V5" s="5" t="inlineStr"/>
+      <c r="W5" s="5" t="inlineStr"/>
+      <c r="X5" s="5" t="inlineStr"/>
+      <c r="Y5" s="5" t="inlineStr"/>
+      <c r="Z5" s="5" t="inlineStr"/>
+      <c r="AA5" s="5" t="inlineStr"/>
+      <c r="AB5" s="6" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>136356</v>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E6" s="5" t="inlineStr">
         <is>
           <t>Balaoa Elementary School</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>TADIAN</t>
         </is>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="n">
+      <c r="H6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="J6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="5" t="n">
         <v>4108545.870713225</v>
       </c>
-      <c r="M6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4" t="inlineStr"/>
-      <c r="O6" s="4" t="inlineStr">
+      <c r="M6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="inlineStr"/>
+      <c r="O6" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4" t="inlineStr"/>
-      <c r="R6" s="4" t="inlineStr"/>
-      <c r="S6" s="4" t="inlineStr"/>
-      <c r="T6" s="4" t="inlineStr"/>
-      <c r="U6" s="4" t="inlineStr"/>
-      <c r="V6" s="4" t="inlineStr"/>
-      <c r="W6" s="4" t="inlineStr"/>
-      <c r="X6" s="4" t="inlineStr"/>
-      <c r="Y6" s="4" t="inlineStr"/>
-      <c r="Z6" s="4" t="inlineStr"/>
-      <c r="AA6" s="4" t="inlineStr"/>
-      <c r="AB6" s="4" t="n"/>
+      <c r="P6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5" t="inlineStr"/>
+      <c r="R6" s="5" t="inlineStr"/>
+      <c r="S6" s="5" t="inlineStr"/>
+      <c r="T6" s="5" t="inlineStr"/>
+      <c r="U6" s="5" t="inlineStr"/>
+      <c r="V6" s="5" t="inlineStr"/>
+      <c r="W6" s="5" t="inlineStr"/>
+      <c r="X6" s="5" t="inlineStr"/>
+      <c r="Y6" s="5" t="inlineStr"/>
+      <c r="Z6" s="5" t="inlineStr"/>
+      <c r="AA6" s="5" t="inlineStr"/>
+      <c r="AB6" s="6" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>136358</v>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Bantey Elementary School</t>
         </is>
       </c>
-      <c r="F7" s="4" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>TADIAN</t>
         </is>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4" t="n">
+      <c r="H7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="J7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
+      <c r="J7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="5" t="n">
         <v>12490756.76</v>
       </c>
-      <c r="M7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4" t="inlineStr"/>
-      <c r="O7" s="4" t="inlineStr">
+      <c r="M7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5" t="inlineStr"/>
+      <c r="O7" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="4" t="inlineStr"/>
-      <c r="R7" s="4" t="inlineStr"/>
-      <c r="S7" s="4" t="inlineStr"/>
-      <c r="T7" s="4" t="inlineStr"/>
-      <c r="U7" s="4" t="inlineStr"/>
-      <c r="V7" s="4" t="inlineStr"/>
-      <c r="W7" s="4" t="inlineStr"/>
-      <c r="X7" s="4" t="inlineStr"/>
-      <c r="Y7" s="4" t="inlineStr"/>
-      <c r="Z7" s="4" t="inlineStr"/>
-      <c r="AA7" s="4" t="inlineStr"/>
-      <c r="AB7" s="4" t="n"/>
+      <c r="P7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5" t="inlineStr"/>
+      <c r="R7" s="5" t="inlineStr"/>
+      <c r="S7" s="5" t="inlineStr"/>
+      <c r="T7" s="5" t="inlineStr"/>
+      <c r="U7" s="5" t="inlineStr"/>
+      <c r="V7" s="5" t="inlineStr"/>
+      <c r="W7" s="5" t="inlineStr"/>
+      <c r="X7" s="5" t="inlineStr"/>
+      <c r="Y7" s="5" t="inlineStr"/>
+      <c r="Z7" s="5" t="inlineStr"/>
+      <c r="AA7" s="5" t="inlineStr"/>
+      <c r="AB7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>136363</v>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>Dacudac Elementary School</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>TADIAN</t>
         </is>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4" t="n">
+      <c r="H8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="4" t="inlineStr">
+      <c r="J8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" s="5" t="n">
         <v>6837175.68</v>
       </c>
-      <c r="M8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4" t="inlineStr"/>
-      <c r="O8" s="4" t="inlineStr">
+      <c r="M8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="inlineStr"/>
+      <c r="O8" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="4" t="inlineStr"/>
-      <c r="R8" s="4" t="inlineStr"/>
-      <c r="S8" s="4" t="inlineStr"/>
-      <c r="T8" s="4" t="inlineStr"/>
-      <c r="U8" s="4" t="inlineStr"/>
-      <c r="V8" s="4" t="inlineStr"/>
-      <c r="W8" s="4" t="inlineStr"/>
-      <c r="X8" s="4" t="inlineStr"/>
-      <c r="Y8" s="4" t="inlineStr"/>
-      <c r="Z8" s="4" t="inlineStr"/>
-      <c r="AA8" s="4" t="inlineStr"/>
-      <c r="AB8" s="4" t="n"/>
+      <c r="P8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5" t="inlineStr"/>
+      <c r="R8" s="5" t="inlineStr"/>
+      <c r="S8" s="5" t="inlineStr"/>
+      <c r="T8" s="5" t="inlineStr"/>
+      <c r="U8" s="5" t="inlineStr"/>
+      <c r="V8" s="5" t="inlineStr"/>
+      <c r="W8" s="5" t="inlineStr"/>
+      <c r="X8" s="5" t="inlineStr"/>
+      <c r="Y8" s="5" t="inlineStr"/>
+      <c r="Z8" s="5" t="inlineStr"/>
+      <c r="AA8" s="5" t="inlineStr"/>
+      <c r="AB8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2020</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>136367</v>
       </c>
-      <c r="E9" s="4" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>Kayan Elementary School</t>
         </is>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>TADIAN</t>
         </is>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="n">
+      <c r="H9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4" t="inlineStr">
+      <c r="J9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L9" s="4" t="n">
+      <c r="L9" s="5" t="n">
         <v>17916759.49</v>
       </c>
-      <c r="M9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4" t="inlineStr"/>
-      <c r="O9" s="4" t="inlineStr">
+      <c r="M9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5" t="inlineStr"/>
+      <c r="O9" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="4" t="inlineStr"/>
-      <c r="R9" s="4" t="inlineStr"/>
-      <c r="S9" s="4" t="inlineStr"/>
-      <c r="T9" s="4" t="inlineStr"/>
-      <c r="U9" s="4" t="inlineStr"/>
-      <c r="V9" s="4" t="inlineStr"/>
-      <c r="W9" s="4" t="inlineStr"/>
-      <c r="X9" s="4" t="inlineStr"/>
-      <c r="Y9" s="4" t="inlineStr"/>
-      <c r="Z9" s="4" t="inlineStr"/>
-      <c r="AA9" s="4" t="inlineStr"/>
-      <c r="AB9" s="4" t="n"/>
+      <c r="P9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5" t="inlineStr"/>
+      <c r="R9" s="5" t="inlineStr"/>
+      <c r="S9" s="5" t="inlineStr"/>
+      <c r="T9" s="5" t="inlineStr"/>
+      <c r="U9" s="5" t="inlineStr"/>
+      <c r="V9" s="5" t="inlineStr"/>
+      <c r="W9" s="5" t="inlineStr"/>
+      <c r="X9" s="5" t="inlineStr"/>
+      <c r="Y9" s="5" t="inlineStr"/>
+      <c r="Z9" s="5" t="inlineStr"/>
+      <c r="AA9" s="5" t="inlineStr"/>
+      <c r="AB9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2021</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>134989</v>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>Bucay CS</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
         <is>
           <t>BUCAY</t>
         </is>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="4" t="inlineStr">
+      <c r="H10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="5" t="n">
         <v>5216538</v>
       </c>
-      <c r="M10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="4" t="inlineStr"/>
-      <c r="O10" s="4" t="inlineStr">
+      <c r="M10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5" t="inlineStr"/>
+      <c r="O10" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="4" t="inlineStr"/>
-      <c r="R10" s="4" t="inlineStr"/>
-      <c r="S10" s="4" t="inlineStr"/>
-      <c r="T10" s="4" t="inlineStr"/>
-      <c r="U10" s="4" t="inlineStr"/>
-      <c r="V10" s="4" t="inlineStr"/>
-      <c r="W10" s="4" t="inlineStr"/>
-      <c r="X10" s="4" t="inlineStr"/>
-      <c r="Y10" s="4" t="inlineStr"/>
-      <c r="Z10" s="4" t="inlineStr"/>
-      <c r="AA10" s="4" t="inlineStr"/>
-      <c r="AB10" s="4" t="n"/>
+      <c r="P10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="5" t="inlineStr"/>
+      <c r="R10" s="5" t="inlineStr"/>
+      <c r="S10" s="5" t="inlineStr"/>
+      <c r="T10" s="5" t="inlineStr"/>
+      <c r="U10" s="5" t="inlineStr"/>
+      <c r="V10" s="5" t="inlineStr"/>
+      <c r="W10" s="5" t="inlineStr"/>
+      <c r="X10" s="5" t="inlineStr"/>
+      <c r="Y10" s="5" t="inlineStr"/>
+      <c r="Z10" s="5" t="inlineStr"/>
+      <c r="AA10" s="5" t="inlineStr"/>
+      <c r="AB10" s="6" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2021</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>135017</v>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="E11" s="5" t="inlineStr">
         <is>
           <t>Dolores CS</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>DOLORES</t>
         </is>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4" t="inlineStr">
+      <c r="H11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="5" t="n">
         <v>4582774</v>
       </c>
-      <c r="M11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="4" t="inlineStr"/>
-      <c r="O11" s="4" t="inlineStr">
+      <c r="M11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="5" t="inlineStr"/>
+      <c r="O11" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="4" t="inlineStr"/>
-      <c r="R11" s="4" t="inlineStr"/>
-      <c r="S11" s="4" t="inlineStr"/>
-      <c r="T11" s="4" t="inlineStr"/>
-      <c r="U11" s="4" t="inlineStr"/>
-      <c r="V11" s="4" t="inlineStr"/>
-      <c r="W11" s="4" t="inlineStr"/>
-      <c r="X11" s="4" t="inlineStr"/>
-      <c r="Y11" s="4" t="inlineStr"/>
-      <c r="Z11" s="4" t="inlineStr"/>
-      <c r="AA11" s="4" t="inlineStr"/>
-      <c r="AB11" s="4" t="n"/>
+      <c r="P11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5" t="inlineStr"/>
+      <c r="R11" s="5" t="inlineStr"/>
+      <c r="S11" s="5" t="inlineStr"/>
+      <c r="T11" s="5" t="inlineStr"/>
+      <c r="U11" s="5" t="inlineStr"/>
+      <c r="V11" s="5" t="inlineStr"/>
+      <c r="W11" s="5" t="inlineStr"/>
+      <c r="X11" s="5" t="inlineStr"/>
+      <c r="Y11" s="5" t="inlineStr"/>
+      <c r="Z11" s="5" t="inlineStr"/>
+      <c r="AA11" s="5" t="inlineStr"/>
+      <c r="AB11" s="6" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2021</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>135103</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>Luba CS</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr">
         <is>
           <t>LUBA</t>
         </is>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4" t="inlineStr">
+      <c r="H12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L12" s="4" t="n">
+      <c r="L12" s="5" t="n">
         <v>5026084</v>
       </c>
-      <c r="M12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4" t="inlineStr"/>
-      <c r="O12" s="4" t="inlineStr">
+      <c r="M12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5" t="inlineStr"/>
+      <c r="O12" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="4" t="inlineStr"/>
-      <c r="R12" s="4" t="inlineStr"/>
-      <c r="S12" s="4" t="inlineStr"/>
-      <c r="T12" s="4" t="inlineStr"/>
-      <c r="U12" s="4" t="inlineStr"/>
-      <c r="V12" s="4" t="inlineStr"/>
-      <c r="W12" s="4" t="inlineStr"/>
-      <c r="X12" s="4" t="inlineStr"/>
-      <c r="Y12" s="4" t="inlineStr"/>
-      <c r="Z12" s="4" t="inlineStr"/>
-      <c r="AA12" s="4" t="inlineStr"/>
-      <c r="AB12" s="4" t="n"/>
+      <c r="P12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5" t="inlineStr"/>
+      <c r="R12" s="5" t="inlineStr"/>
+      <c r="S12" s="5" t="inlineStr"/>
+      <c r="T12" s="5" t="inlineStr"/>
+      <c r="U12" s="5" t="inlineStr"/>
+      <c r="V12" s="5" t="inlineStr"/>
+      <c r="W12" s="5" t="inlineStr"/>
+      <c r="X12" s="5" t="inlineStr"/>
+      <c r="Y12" s="5" t="inlineStr"/>
+      <c r="Z12" s="5" t="inlineStr"/>
+      <c r="AA12" s="5" t="inlineStr"/>
+      <c r="AB12" s="6" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2021</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="5" t="n">
         <v>135435</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="inlineStr">
         <is>
           <t>Bokod CS</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" s="5" t="inlineStr">
         <is>
           <t>BOKOD</t>
         </is>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4" t="n">
+      <c r="H13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4" t="inlineStr">
+      <c r="J13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L13" s="4" t="n">
+      <c r="L13" s="5" t="n">
         <v>16817332</v>
       </c>
-      <c r="M13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4" t="inlineStr"/>
-      <c r="O13" s="4" t="inlineStr">
+      <c r="M13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="5" t="inlineStr"/>
+      <c r="O13" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="4" t="inlineStr"/>
-      <c r="R13" s="4" t="inlineStr"/>
-      <c r="S13" s="4" t="inlineStr"/>
-      <c r="T13" s="4" t="inlineStr"/>
-      <c r="U13" s="4" t="inlineStr"/>
-      <c r="V13" s="4" t="inlineStr"/>
-      <c r="W13" s="4" t="inlineStr"/>
-      <c r="X13" s="4" t="inlineStr"/>
-      <c r="Y13" s="4" t="inlineStr"/>
-      <c r="Z13" s="4" t="inlineStr"/>
-      <c r="AA13" s="4" t="inlineStr"/>
-      <c r="AB13" s="4" t="n"/>
+      <c r="P13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="5" t="inlineStr"/>
+      <c r="R13" s="5" t="inlineStr"/>
+      <c r="S13" s="5" t="inlineStr"/>
+      <c r="T13" s="5" t="inlineStr"/>
+      <c r="U13" s="5" t="inlineStr"/>
+      <c r="V13" s="5" t="inlineStr"/>
+      <c r="W13" s="5" t="inlineStr"/>
+      <c r="X13" s="5" t="inlineStr"/>
+      <c r="Y13" s="5" t="inlineStr"/>
+      <c r="Z13" s="5" t="inlineStr"/>
+      <c r="AA13" s="5" t="inlineStr"/>
+      <c r="AB13" s="6" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2021</t>
         </is>
       </c>
-      <c r="B14" s="4" t="inlineStr">
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="5" t="n">
         <v>136202</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="E14" s="5" t="inlineStr">
         <is>
           <t>Bauko Central School</t>
         </is>
       </c>
-      <c r="F14" s="4" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>BAUKO</t>
         </is>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4" t="n">
+      <c r="H14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="J14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="4" t="inlineStr">
+      <c r="J14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="5" t="n">
         <v>38640021</v>
       </c>
-      <c r="M14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" s="4" t="inlineStr"/>
-      <c r="O14" s="4" t="inlineStr">
+      <c r="M14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5" t="inlineStr"/>
+      <c r="O14" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="4" t="inlineStr"/>
-      <c r="R14" s="4" t="inlineStr"/>
-      <c r="S14" s="4" t="inlineStr"/>
-      <c r="T14" s="4" t="inlineStr"/>
-      <c r="U14" s="4" t="inlineStr"/>
-      <c r="V14" s="4" t="inlineStr"/>
-      <c r="W14" s="4" t="inlineStr"/>
-      <c r="X14" s="4" t="inlineStr"/>
-      <c r="Y14" s="4" t="inlineStr"/>
-      <c r="Z14" s="4" t="inlineStr"/>
-      <c r="AA14" s="4" t="inlineStr"/>
-      <c r="AB14" s="4" t="n"/>
+      <c r="P14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="5" t="inlineStr"/>
+      <c r="R14" s="5" t="inlineStr"/>
+      <c r="S14" s="5" t="inlineStr"/>
+      <c r="T14" s="5" t="inlineStr"/>
+      <c r="U14" s="5" t="inlineStr"/>
+      <c r="V14" s="5" t="inlineStr"/>
+      <c r="W14" s="5" t="inlineStr"/>
+      <c r="X14" s="5" t="inlineStr"/>
+      <c r="Y14" s="5" t="inlineStr"/>
+      <c r="Z14" s="5" t="inlineStr"/>
+      <c r="AA14" s="5" t="inlineStr"/>
+      <c r="AB14" s="6" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="A15" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2022</t>
         </is>
       </c>
-      <c r="B15" s="4" t="inlineStr">
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="5" t="n">
         <v>136239</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
+      <c r="E15" s="5" t="inlineStr">
         <is>
           <t>Dandanac Elementary School</t>
         </is>
       </c>
-      <c r="F15" s="4" t="inlineStr">
+      <c r="F15" s="5" t="inlineStr">
         <is>
           <t>BESAO</t>
         </is>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4" t="n">
+      <c r="H15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" s="4" t="inlineStr">
+      <c r="J15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="5" t="n">
         <v>14828997.48</v>
       </c>
-      <c r="M15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" s="4" t="n">
+      <c r="M15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="5" t="n">
         <v>147777975.49</v>
       </c>
-      <c r="O15" s="4" t="inlineStr">
+      <c r="O15" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="4" t="inlineStr">
+      <c r="P15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="5" t="inlineStr">
         <is>
           <t>5/31/2023</t>
         </is>
       </c>
-      <c r="R15" s="4" t="inlineStr">
+      <c r="R15" s="5" t="inlineStr">
         <is>
           <t>August 10, 2023</t>
         </is>
       </c>
-      <c r="S15" s="4" t="inlineStr">
+      <c r="S15" s="5" t="inlineStr">
         <is>
           <t>INF2022GAB001</t>
         </is>
       </c>
-      <c r="T15" s="4" t="inlineStr">
+      <c r="T15" s="5" t="inlineStr">
         <is>
           <t>INF2022GAB001</t>
         </is>
       </c>
-      <c r="U15" s="4" t="inlineStr">
+      <c r="U15" s="5" t="inlineStr">
         <is>
           <t>7/30/2022</t>
         </is>
       </c>
-      <c r="V15" s="5" t="n">
+      <c r="V15" s="7" t="n">
         <v>44600</v>
       </c>
-      <c r="W15" s="4" t="inlineStr">
+      <c r="W15" s="5" t="inlineStr">
         <is>
           <t>8/15/2022</t>
         </is>
       </c>
-      <c r="X15" s="4" t="inlineStr">
+      <c r="X15" s="5" t="inlineStr">
         <is>
           <t>Sept 19, 2022</t>
         </is>
       </c>
-      <c r="Y15" s="4" t="inlineStr">
+      <c r="Y15" s="5" t="inlineStr">
         <is>
           <t>11/25/2022</t>
         </is>
       </c>
-      <c r="Z15" s="4" t="inlineStr">
+      <c r="Z15" s="5" t="inlineStr">
         <is>
           <t>JM-MAS Construction &amp; Gen. MDSE.</t>
         </is>
       </c>
-      <c r="AA15" s="4" t="inlineStr"/>
-      <c r="AB15" s="4" t="n"/>
+      <c r="AA15" s="5" t="inlineStr"/>
+      <c r="AB15" s="6" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2022</t>
         </is>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>Mt. Province</t>
         </is>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="5" t="n">
         <v>136342</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>Ambasing Elementary School</t>
         </is>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>SAGADA</t>
         </is>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="4" t="n">
+      <c r="H16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="4" t="inlineStr">
+      <c r="J16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="5" t="inlineStr">
         <is>
           <t>Rehabilitation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L16" s="4" t="n">
+      <c r="L16" s="5" t="n">
         <v>37800000</v>
       </c>
-      <c r="M16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="4" t="n">
+      <c r="M16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="n">
         <v>37720000</v>
       </c>
-      <c r="O16" s="4" t="inlineStr">
+      <c r="O16" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="4" t="inlineStr">
+      <c r="P16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5" t="inlineStr">
         <is>
           <t>7/30/2023</t>
         </is>
       </c>
-      <c r="R16" s="4" t="inlineStr">
+      <c r="R16" s="5" t="inlineStr">
         <is>
           <t>July 12, 2024</t>
         </is>
       </c>
-      <c r="S16" s="4" t="inlineStr">
+      <c r="S16" s="5" t="inlineStr">
         <is>
           <t>INF2022GAB002</t>
         </is>
       </c>
-      <c r="T16" s="4" t="inlineStr">
+      <c r="T16" s="5" t="inlineStr">
         <is>
           <t>INF2022GAB002</t>
         </is>
       </c>
-      <c r="U16" s="4" t="inlineStr">
+      <c r="U16" s="5" t="inlineStr">
         <is>
           <t>7/30/2023</t>
         </is>
       </c>
-      <c r="V16" s="5" t="n">
+      <c r="V16" s="7" t="n">
         <v>44600</v>
       </c>
-      <c r="W16" s="4" t="inlineStr">
+      <c r="W16" s="5" t="inlineStr">
         <is>
           <t>8/15/2022</t>
         </is>
       </c>
-      <c r="X16" s="4" t="inlineStr">
+      <c r="X16" s="5" t="inlineStr">
         <is>
           <t>Sept 19, 2022</t>
         </is>
       </c>
-      <c r="Y16" s="4" t="inlineStr">
+      <c r="Y16" s="5" t="inlineStr">
         <is>
           <t>11/25/2022</t>
         </is>
       </c>
-      <c r="Z16" s="4" t="inlineStr">
+      <c r="Z16" s="5" t="inlineStr">
         <is>
           <t>BAJE CONSTRUCTIOIN</t>
         </is>
       </c>
-      <c r="AA16" s="4" t="inlineStr"/>
-      <c r="AB16" s="4" t="n"/>
+      <c r="AA16" s="5" t="inlineStr"/>
+      <c r="AB16" s="6" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2023</t>
         </is>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>Baguio City</t>
         </is>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <v>136382</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="E17" s="5" t="inlineStr">
         <is>
           <t>Baguio Central School</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="5" t="inlineStr">
         <is>
           <t>BAGUIO CITY</t>
         </is>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="4" t="inlineStr">
+      <c r="H17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="5" t="inlineStr">
         <is>
           <t>Restoration &amp; Conservation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L17" s="4" t="n">
+      <c r="L17" s="5" t="n">
         <v>41223103.23</v>
       </c>
-      <c r="M17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="4" t="n">
+      <c r="M17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5" t="n">
         <v>40014561</v>
       </c>
-      <c r="O17" s="4" t="inlineStr">
+      <c r="O17" s="5" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="P17" s="4" t="n">
+      <c r="P17" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="Q17" s="4" t="inlineStr">
+      <c r="Q17" s="5" t="inlineStr">
         <is>
           <t>November 5,2025</t>
         </is>
       </c>
-      <c r="R17" s="4" t="inlineStr"/>
-      <c r="S17" s="4" t="inlineStr">
+      <c r="R17" s="5" t="inlineStr"/>
+      <c r="S17" s="5" t="inlineStr">
         <is>
           <t>No.027,s.2023</t>
         </is>
       </c>
-      <c r="T17" s="4" t="inlineStr">
+      <c r="T17" s="5" t="inlineStr">
         <is>
           <t>No.027,s.2023</t>
         </is>
       </c>
-      <c r="U17" s="4" t="inlineStr">
+      <c r="U17" s="5" t="inlineStr">
         <is>
           <t>December 9, 2023</t>
         </is>
       </c>
-      <c r="V17" s="4" t="inlineStr">
+      <c r="V17" s="5" t="inlineStr">
         <is>
           <t>December 15, 2023</t>
         </is>
       </c>
-      <c r="W17" s="4" t="inlineStr">
+      <c r="W17" s="5" t="inlineStr">
         <is>
           <t>December 29, 2023</t>
         </is>
       </c>
-      <c r="X17" s="4" t="inlineStr">
+      <c r="X17" s="5" t="inlineStr">
         <is>
           <t>January 18, 2024</t>
         </is>
       </c>
-      <c r="Y17" s="4" t="inlineStr">
+      <c r="Y17" s="5" t="inlineStr">
         <is>
           <t>February 20, 2024</t>
         </is>
       </c>
-      <c r="Z17" s="4" t="inlineStr">
+      <c r="Z17" s="5" t="inlineStr">
         <is>
           <t>EZRAH Construction Services/HGW=3 Engineering and Construction</t>
         </is>
       </c>
-      <c r="AA17" s="4" t="inlineStr">
+      <c r="AA17" s="5" t="inlineStr">
         <is>
           <t>Project suspended as to LGU's order while the submission and approval of Conservation Management Plan and Building Permit</t>
         </is>
       </c>
-      <c r="AB17" s="4" t="n"/>
+      <c r="AB17" s="6" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2023</t>
         </is>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="C18" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="5" t="n">
         <v>135402</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="E18" s="5" t="inlineStr">
         <is>
           <t>Bagu ES</t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>BAKUN</t>
         </is>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="4" t="n">
+      <c r="H18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" s="4" t="inlineStr">
+      <c r="J18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="5" t="inlineStr">
         <is>
           <t>Restoration &amp; Conservation of Gabaldon Building</t>
         </is>
       </c>
-      <c r="L18" s="4" t="n">
+      <c r="L18" s="5" t="n">
         <v>10000000</v>
       </c>
-      <c r="M18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N18" s="4" t="n">
+      <c r="M18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="5" t="n">
         <v>10000000</v>
       </c>
-      <c r="O18" s="4" t="inlineStr">
+      <c r="O18" s="5" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="P18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="4" t="inlineStr">
+      <c r="P18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="5" t="inlineStr">
         <is>
           <t>9/17/2024</t>
         </is>
       </c>
-      <c r="R18" s="4" t="inlineStr">
+      <c r="R18" s="5" t="inlineStr">
         <is>
           <t>12/13/2024</t>
         </is>
       </c>
-      <c r="S18" s="4" t="inlineStr">
+      <c r="S18" s="5" t="inlineStr">
         <is>
           <t>GAB-2023-01</t>
         </is>
       </c>
-      <c r="T18" s="4" t="inlineStr">
+      <c r="T18" s="5" t="inlineStr">
         <is>
           <t>GAB-2023-02</t>
         </is>
       </c>
-      <c r="U18" s="5" t="n">
+      <c r="U18" s="7" t="n">
         <v>45051</v>
       </c>
-      <c r="V18" s="5" t="n">
+      <c r="V18" s="7" t="n">
         <v>45265</v>
       </c>
-      <c r="W18" s="4" t="inlineStr">
+      <c r="W18" s="5" t="inlineStr">
         <is>
           <t>5/25/2023</t>
         </is>
       </c>
-      <c r="X18" s="4" t="inlineStr">
+      <c r="X18" s="5" t="inlineStr">
         <is>
           <t>7/28/2023</t>
         </is>
       </c>
-      <c r="Y18" s="4" t="inlineStr">
+      <c r="Y18" s="5" t="inlineStr">
         <is>
           <t>9/18/2023</t>
         </is>
       </c>
-      <c r="Z18" s="4" t="inlineStr">
+      <c r="Z18" s="5" t="inlineStr">
         <is>
           <t>SCA JR BUILDERS</t>
         </is>
       </c>
-      <c r="AA18" s="4" t="inlineStr"/>
-      <c r="AB18" s="4" t="n"/>
+      <c r="AA18" s="5" t="inlineStr"/>
+      <c r="AB18" s="6" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2024</t>
         </is>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="5" t="n">
         <v>134979</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="E19" s="5" t="inlineStr">
         <is>
           <t>Bangued West CS</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>BANGUED (Capital)</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="G19" s="5" t="inlineStr">
         <is>
           <t>Lone</t>
         </is>
       </c>
-      <c r="H19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="4" t="n">
+      <c r="H19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="J19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" s="4" t="inlineStr">
+      <c r="J19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5" t="inlineStr">
         <is>
           <t>Conservation and Restoration of Gabaldon School Building</t>
         </is>
       </c>
-      <c r="L19" s="4" t="n">
+      <c r="L19" s="5" t="n">
         <v>12905610</v>
       </c>
-      <c r="M19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" s="4" t="n">
+      <c r="M19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5" t="n">
         <v>12887697.3</v>
       </c>
-      <c r="O19" s="4" t="inlineStr">
+      <c r="O19" s="5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="P19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="4" t="inlineStr">
+      <c r="P19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="5" t="inlineStr">
         <is>
           <t>November 5, 2024</t>
         </is>
       </c>
-      <c r="R19" s="4" t="inlineStr">
+      <c r="R19" s="5" t="inlineStr">
         <is>
           <t>November 5, 2024</t>
         </is>
       </c>
-      <c r="S19" s="4" t="inlineStr">
+      <c r="S19" s="5" t="inlineStr">
         <is>
           <t>CAR-ABRA-2024-04-006</t>
         </is>
       </c>
-      <c r="T19" s="4" t="inlineStr">
+      <c r="T19" s="5" t="inlineStr">
         <is>
           <t>2024-07-007</t>
         </is>
       </c>
-      <c r="U19" s="4" t="inlineStr">
+      <c r="U19" s="5" t="inlineStr">
         <is>
           <t>April 17, 2024</t>
         </is>
       </c>
-      <c r="V19" s="4" t="inlineStr">
+      <c r="V19" s="5" t="inlineStr">
         <is>
           <t>April 24, 2024</t>
         </is>
       </c>
-      <c r="W19" s="4" t="inlineStr">
+      <c r="W19" s="5" t="inlineStr">
         <is>
           <t>May 7, 2024</t>
         </is>
       </c>
-      <c r="X19" s="4" t="inlineStr">
+      <c r="X19" s="5" t="inlineStr">
         <is>
           <t>May 16, 2024</t>
         </is>
       </c>
-      <c r="Y19" s="4" t="inlineStr">
+      <c r="Y19" s="5" t="inlineStr">
         <is>
           <t>July 8, 2024</t>
         </is>
       </c>
-      <c r="Z19" s="4" t="inlineStr">
+      <c r="Z19" s="5" t="inlineStr">
         <is>
           <t>BAJE CONSTRUCTIOIN</t>
         </is>
       </c>
-      <c r="AA19" s="4" t="inlineStr"/>
-      <c r="AB19" s="4" t="n"/>
+      <c r="AA19" s="5" t="inlineStr"/>
+      <c r="AB19" s="6" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2024</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr">
+      <c r="B20" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="C20" s="5" t="inlineStr">
         <is>
           <t>Abra</t>
         </is>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="5" t="n">
         <v>135223</v>
       </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="E20" s="5" t="inlineStr">
         <is>
           <t>San Juan CS</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" s="5" t="inlineStr">
         <is>
           <t>SAN JUAN</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr">
+      <c r="G20" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Lone </t>
         </is>
       </c>
-      <c r="H20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="4" t="n">
+      <c r="H20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="J20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="4" t="inlineStr">
+      <c r="J20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5" t="inlineStr">
         <is>
           <t>Conservation and Restoration of Gabaldon School Building</t>
         </is>
       </c>
-      <c r="L20" s="4" t="n">
+      <c r="L20" s="5" t="n">
         <v>25000000</v>
       </c>
-      <c r="M20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" s="4" t="n">
+      <c r="M20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5" t="n">
         <v>24988913.87</v>
       </c>
-      <c r="O20" s="4" t="inlineStr">
+      <c r="O20" s="5" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="P20" s="4" t="n">
+      <c r="P20" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="Q20" s="4" t="inlineStr">
+      <c r="Q20" s="5" t="inlineStr">
         <is>
           <t>February 3, 2025</t>
         </is>
       </c>
-      <c r="R20" s="4" t="inlineStr"/>
-      <c r="S20" s="4" t="inlineStr">
+      <c r="R20" s="5" t="inlineStr"/>
+      <c r="S20" s="5" t="inlineStr">
         <is>
           <t>CAR-ABRA-2024-04-006</t>
         </is>
       </c>
-      <c r="T20" s="4" t="inlineStr">
+      <c r="T20" s="5" t="inlineStr">
         <is>
           <t>2024-07-007</t>
         </is>
       </c>
-      <c r="U20" s="4" t="inlineStr">
+      <c r="U20" s="5" t="inlineStr">
         <is>
           <t>April 17, 2024</t>
         </is>
       </c>
-      <c r="V20" s="4" t="inlineStr">
+      <c r="V20" s="5" t="inlineStr">
         <is>
           <t>April 24, 2024</t>
         </is>
       </c>
-      <c r="W20" s="4" t="inlineStr">
+      <c r="W20" s="5" t="inlineStr">
         <is>
           <t>May 7, 2024</t>
         </is>
       </c>
-      <c r="X20" s="4" t="inlineStr">
+      <c r="X20" s="5" t="inlineStr">
         <is>
           <t>May 16, 2024</t>
         </is>
       </c>
-      <c r="Y20" s="4" t="inlineStr">
+      <c r="Y20" s="5" t="inlineStr">
         <is>
           <t>July 8, 2024</t>
         </is>
       </c>
-      <c r="Z20" s="4" t="inlineStr">
+      <c r="Z20" s="5" t="inlineStr">
         <is>
           <t>BAJE CONSTRUCTIOIN</t>
         </is>
       </c>
-      <c r="AA20" s="4" t="inlineStr"/>
-      <c r="AB20" s="4" t="n"/>
+      <c r="AA20" s="5" t="inlineStr"/>
+      <c r="AB20" s="6" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2024</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C21" s="4" t="inlineStr">
+      <c r="C21" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="5" t="n">
         <v>135438</v>
       </c>
-      <c r="E21" s="4" t="inlineStr">
+      <c r="E21" s="5" t="inlineStr">
         <is>
           <t>Daklan ES</t>
         </is>
       </c>
-      <c r="F21" s="4" t="inlineStr">
+      <c r="F21" s="5" t="inlineStr">
         <is>
           <t>BOKOD</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr">
+      <c r="G21" s="5" t="inlineStr">
         <is>
           <t>Lone</t>
         </is>
       </c>
-      <c r="H21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4" t="n">
+      <c r="H21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="J21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
+      <c r="J21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5" t="inlineStr">
         <is>
           <t>Conservation and Restoration of Gabaldon School Building</t>
         </is>
       </c>
-      <c r="L21" s="4" t="n">
+      <c r="L21" s="5" t="n">
         <v>19094390</v>
       </c>
-      <c r="M21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" s="4" t="n">
+      <c r="M21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="5" t="n">
         <v>18378750</v>
       </c>
-      <c r="O21" s="4" t="inlineStr">
+      <c r="O21" s="5" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="P21" s="4" t="n">
+      <c r="P21" s="5" t="n">
         <v>0.45</v>
       </c>
-      <c r="Q21" s="4" t="inlineStr">
+      <c r="Q21" s="5" t="inlineStr">
         <is>
           <t>August 5,2025</t>
         </is>
       </c>
-      <c r="R21" s="4" t="inlineStr"/>
-      <c r="S21" s="4" t="inlineStr">
+      <c r="R21" s="5" t="inlineStr"/>
+      <c r="S21" s="5" t="inlineStr">
         <is>
           <t>GAB-2024-02</t>
         </is>
       </c>
-      <c r="T21" s="4" t="inlineStr">
+      <c r="T21" s="5" t="inlineStr">
         <is>
           <t>GAB-2024-02</t>
         </is>
       </c>
-      <c r="U21" s="4" t="inlineStr">
+      <c r="U21" s="5" t="inlineStr">
         <is>
           <t>MAY 29. 2024</t>
         </is>
       </c>
-      <c r="V21" s="5" t="n">
+      <c r="V21" s="7" t="n">
         <v>45571</v>
       </c>
-      <c r="W21" s="4" t="inlineStr">
+      <c r="W21" s="5" t="inlineStr">
         <is>
           <t>6/24/2024</t>
         </is>
       </c>
-      <c r="X21" s="4" t="inlineStr">
+      <c r="X21" s="5" t="inlineStr">
         <is>
           <t>September 26, 2024</t>
         </is>
       </c>
-      <c r="Y21" s="4" t="inlineStr">
+      <c r="Y21" s="5" t="inlineStr">
         <is>
           <t>October 31, 2024</t>
         </is>
       </c>
-      <c r="Z21" s="4" t="inlineStr">
+      <c r="Z21" s="5" t="inlineStr">
         <is>
           <t>MHIGS CONSTRUCTION</t>
         </is>
       </c>
-      <c r="AA21" s="4" t="inlineStr"/>
-      <c r="AB21" s="4" t="n"/>
+      <c r="AA21" s="5" t="inlineStr"/>
+      <c r="AB21" s="6" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2024</t>
         </is>
       </c>
-      <c r="B22" s="4" t="inlineStr">
+      <c r="B22" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr">
+      <c r="C22" s="5" t="inlineStr">
         <is>
           <t>Benguet</t>
         </is>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="5" t="n">
         <v>135619</v>
       </c>
-      <c r="E22" s="4" t="inlineStr">
+      <c r="E22" s="5" t="inlineStr">
         <is>
           <t>Bekkel ES</t>
         </is>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="F22" s="5" t="inlineStr">
         <is>
           <t>LA TRINIDAD (Capital)</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="G22" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Lone </t>
         </is>
       </c>
-      <c r="H22" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4" t="n">
+      <c r="H22" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="J22" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
+      <c r="J22" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="5" t="inlineStr">
         <is>
           <t>Conservation and Restoration of Gabaldon School Building</t>
         </is>
       </c>
-      <c r="L22" s="4" t="n">
+      <c r="L22" s="5" t="n">
         <v>23919100</v>
       </c>
-      <c r="M22" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N22" s="4" t="n">
+      <c r="M22" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" s="5" t="n">
         <v>22932793.89</v>
       </c>
-      <c r="O22" s="4" t="inlineStr">
+      <c r="O22" s="5" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="P22" s="4" t="n">
+      <c r="P22" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="Q22" s="4" t="inlineStr">
+      <c r="Q22" s="5" t="inlineStr">
         <is>
           <t>August 5,2025</t>
         </is>
       </c>
-      <c r="R22" s="4" t="inlineStr"/>
-      <c r="S22" s="4" t="inlineStr">
+      <c r="R22" s="5" t="inlineStr"/>
+      <c r="S22" s="5" t="inlineStr">
         <is>
           <t>GAB-2024-01</t>
         </is>
       </c>
-      <c r="T22" s="4" t="inlineStr">
+      <c r="T22" s="5" t="inlineStr">
         <is>
           <t>GAB-2024-01</t>
         </is>
       </c>
-      <c r="U22" s="4" t="inlineStr">
+      <c r="U22" s="5" t="inlineStr">
         <is>
           <t>MAY 29. 2024</t>
         </is>
       </c>
-      <c r="V22" s="5" t="n">
+      <c r="V22" s="7" t="n">
         <v>45571</v>
       </c>
-      <c r="W22" s="4" t="inlineStr">
+      <c r="W22" s="5" t="inlineStr">
         <is>
           <t>6/24/2024</t>
         </is>
       </c>
-      <c r="X22" s="4" t="inlineStr">
+      <c r="X22" s="5" t="inlineStr">
         <is>
           <t>September 26, 2024</t>
         </is>
       </c>
-      <c r="Y22" s="4" t="inlineStr">
+      <c r="Y22" s="5" t="inlineStr">
         <is>
           <t>October 31, 2024</t>
         </is>
       </c>
-      <c r="Z22" s="4" t="inlineStr">
+      <c r="Z22" s="5" t="inlineStr">
         <is>
           <t>JRF ANGOYNA GENERAL CONSTRUCTION/REKO KONSTRUCT-JV</t>
         </is>
       </c>
-      <c r="AA22" s="4" t="inlineStr"/>
-      <c r="AB22" s="4" t="n"/>
+      <c r="AA22" s="5" t="inlineStr"/>
+      <c r="AB22" s="6" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
         <is>
           <t>GABALDON 2024</t>
         </is>
       </c>
-      <c r="B23" s="4" t="inlineStr">
+      <c r="B23" s="5" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
+      <c r="C23" s="5" t="inlineStr">
         <is>
           <t>Ifugao</t>
         </is>
       </c>
-      <c r="D23" s="4" t="n">
+      <c r="D23" s="5" t="n">
         <v>220020</v>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="E23" s="5" t="inlineStr">
         <is>
           <t>Ifugao SPED Center</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="F23" s="5" t="inlineStr">
         <is>
           <t>LAGAWE (Capital)</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr">
+      <c r="G23" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Lone </t>
         </is>
       </c>
-      <c r="H23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4" t="n">
+      <c r="H23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="J23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
+      <c r="J23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5" t="inlineStr">
         <is>
           <t>Conservation and Restoration of Gabaldon School Building</t>
         </is>
       </c>
-      <c r="L23" s="4" t="n">
+      <c r="L23" s="5" t="n">
         <v>34222823.15</v>
       </c>
-      <c r="M23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N23" s="4" t="inlineStr"/>
-      <c r="O23" s="4" t="inlineStr">
+      <c r="M23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5" t="inlineStr"/>
+      <c r="O23" s="5" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="P23" s="4" t="n">
+      <c r="P23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="4" t="inlineStr"/>
-      <c r="R23" s="4" t="inlineStr"/>
-      <c r="S23" s="4" t="inlineStr"/>
-      <c r="T23" s="4" t="inlineStr"/>
-      <c r="U23" s="4" t="inlineStr"/>
-      <c r="V23" s="4" t="inlineStr"/>
-      <c r="W23" s="4" t="inlineStr"/>
-      <c r="X23" s="4" t="inlineStr"/>
-      <c r="Y23" s="4" t="inlineStr"/>
-      <c r="Z23" s="4" t="inlineStr"/>
-      <c r="AA23" s="4" t="inlineStr">
+      <c r="Q23" s="5" t="inlineStr"/>
+      <c r="R23" s="5" t="inlineStr"/>
+      <c r="S23" s="5" t="inlineStr"/>
+      <c r="T23" s="5" t="inlineStr"/>
+      <c r="U23" s="5" t="inlineStr"/>
+      <c r="V23" s="5" t="inlineStr"/>
+      <c r="W23" s="5" t="inlineStr"/>
+      <c r="X23" s="5" t="inlineStr"/>
+      <c r="Y23" s="5" t="inlineStr"/>
+      <c r="Z23" s="5" t="inlineStr"/>
+      <c r="AA23" s="5" t="inlineStr">
         <is>
           <t>Ongoing Preparation of Plans, POW and CMP</t>
         </is>
       </c>
-      <c r="AB23" s="4" t="n"/>
+      <c r="AB23" s="6" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>